<commit_message>
fix command builder and test data
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jammytan/Documents/STV-Project/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C968A1-0AB5-E54E-8EFD-0E4EFDD69590}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C43BB2-DBF4-6B4A-BE0A-02A54D66A789}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="3" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="4" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="354">
   <si>
     <t>component</t>
   </si>
@@ -1451,6 +1451,49 @@
   </si>
   <si>
     <t>list_delete_list_btn</t>
+  </si>
+  <si>
+    <t>//*[@class='android.widget.LinearLayout' and ./android.widget.TextView[@text='${NAME}']</t>
+  </si>
+  <si>
+    <t>${NAME}</t>
+  </si>
+  <si>
+    <t>${INDEX}</t>
+  </si>
+  <si>
+    <t>${HOURS}</t>
+  </si>
+  <si>
+    <t>${MINUTES}</t>
+  </si>
+  <si>
+    <t>${DATE}</t>
+  </si>
+  <si>
+    <t>${YEAR}</t>
+  </si>
+  <si>
+    <r>
+      <t>//*[@class='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>android.widget.LinearLayout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' and @index='${INDEX}']</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1674,6 +1717,25 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1683,39 +1745,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2049,8 +2092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EF6FCC3-78DA-E74D-BF53-4A0FCE774DC3}">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="113" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21:E22"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -2076,7 +2119,7 @@
       <c r="D1" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="25" t="s">
         <v>292</v>
       </c>
     </row>
@@ -2087,7 +2130,7 @@
       <c r="B2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="29" t="s">
         <v>291</v>
       </c>
     </row>
@@ -2164,10 +2207,10 @@
         <v>140</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>109</v>
+        <v>347</v>
       </c>
       <c r="E10" s="30"/>
     </row>
@@ -2179,7 +2222,7 @@
         <v>138</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>139</v>
+        <v>348</v>
       </c>
       <c r="E11" s="30"/>
     </row>
@@ -2187,22 +2230,22 @@
       <c r="A12" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>110</v>
+      <c r="B12" s="11" t="s">
+        <v>346</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E12" s="33"/>
+        <v>347</v>
+      </c>
+      <c r="E12" s="31"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="32" t="s">
         <v>272</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="34"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
@@ -2211,7 +2254,7 @@
       <c r="B14" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="35" t="s">
         <v>293</v>
       </c>
     </row>
@@ -2222,19 +2265,19 @@
       <c r="B15" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="37"/>
+      <c r="E15" s="35"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
         <v>60</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>196</v>
+        <v>353</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="E16" s="37"/>
+        <v>348</v>
+      </c>
+      <c r="E16" s="35"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="11" t="s">
@@ -2246,7 +2289,7 @@
       <c r="D17" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E17" s="37"/>
+      <c r="E17" s="35"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
@@ -2255,7 +2298,7 @@
       <c r="B18" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="37"/>
+      <c r="E18" s="35"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
@@ -2264,16 +2307,16 @@
       <c r="B19" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="37"/>
+      <c r="E19" s="35"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="32" t="s">
         <v>287</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="27"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="34"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
@@ -2282,7 +2325,7 @@
       <c r="B21" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="32" t="s">
+      <c r="E21" s="29" t="s">
         <v>294</v>
       </c>
     </row>
@@ -2293,16 +2336,16 @@
       <c r="B22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="33"/>
+      <c r="E22" s="31"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="32" t="s">
         <v>282</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="27"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="34"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="14" t="s">
@@ -2311,7 +2354,7 @@
       <c r="B24" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="29" t="s">
         <v>295</v>
       </c>
     </row>
@@ -2340,16 +2383,16 @@
       <c r="B27" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="E27" s="33"/>
+      <c r="E27" s="31"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="32" t="s">
         <v>277</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="27"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="34"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="11" t="s">
@@ -2358,7 +2401,7 @@
       <c r="B29" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="E29" s="32" t="s">
+      <c r="E29" s="29" t="s">
         <v>296</v>
       </c>
     </row>
@@ -2397,18 +2440,18 @@
         <v>110</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E33" s="33"/>
+        <v>347</v>
+      </c>
+      <c r="E33" s="31"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="32" t="s">
         <v>278</v>
       </c>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="27"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="34"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="23" t="s">
@@ -2418,7 +2461,7 @@
         <v>261</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="E35" s="32" t="s">
+      <c r="E35" s="29" t="s">
         <v>297</v>
       </c>
     </row>
@@ -2466,18 +2509,18 @@
         <v>110</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E40" s="33"/>
+        <v>347</v>
+      </c>
+      <c r="E40" s="31"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="28" t="s">
+      <c r="A41" s="36" t="s">
         <v>279</v>
       </c>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="36"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="38"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="23" t="s">
@@ -2487,7 +2530,7 @@
         <v>263</v>
       </c>
       <c r="C42" s="7"/>
-      <c r="E42" s="32" t="s">
+      <c r="E42" s="29" t="s">
         <v>298</v>
       </c>
     </row>
@@ -2526,7 +2569,7 @@
         <v>138</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>139</v>
+        <v>348</v>
       </c>
       <c r="E46" s="30"/>
     </row>
@@ -2538,18 +2581,18 @@
         <v>110</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E47" s="33"/>
+        <v>347</v>
+      </c>
+      <c r="E47" s="31"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="25" t="s">
+      <c r="A48" s="32" t="s">
         <v>280</v>
       </c>
-      <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27"/>
+      <c r="B48" s="33"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="34"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="23" t="s">
@@ -2559,7 +2602,7 @@
         <v>264</v>
       </c>
       <c r="C49" s="7"/>
-      <c r="E49" s="32" t="s">
+      <c r="E49" s="29" t="s">
         <v>299</v>
       </c>
     </row>
@@ -2607,18 +2650,18 @@
         <v>110</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E54" s="33"/>
+        <v>347</v>
+      </c>
+      <c r="E54" s="31"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="25" t="s">
+      <c r="A55" s="32" t="s">
         <v>281</v>
       </c>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="27"/>
+      <c r="B55" s="33"/>
+      <c r="C55" s="33"/>
+      <c r="D55" s="33"/>
+      <c r="E55" s="34"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="23" t="s">
@@ -2631,7 +2674,7 @@
       <c r="D56" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E56" s="32" t="s">
+      <c r="E56" s="29" t="s">
         <v>302</v>
       </c>
     </row>
@@ -2652,7 +2695,7 @@
         <v>138</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>139</v>
+        <v>348</v>
       </c>
       <c r="E58" s="30"/>
     </row>
@@ -2664,7 +2707,7 @@
         <v>110</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>109</v>
+        <v>347</v>
       </c>
       <c r="E59" s="30"/>
     </row>
@@ -2676,12 +2719,13 @@
         <v>110</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>109</v>
+        <v>347</v>
       </c>
       <c r="E60" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A55:E55"/>
     <mergeCell ref="E42:E47"/>
     <mergeCell ref="E49:E54"/>
     <mergeCell ref="E56:E60"/>
@@ -2698,7 +2742,6 @@
     <mergeCell ref="A41:E41"/>
     <mergeCell ref="E35:E40"/>
     <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A55:E55"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E21:E22" r:id="rId1" display="ConfirmDelete.png" xr:uid="{E7D51FE5-38A8-ED48-AB1B-5439A79F0F01}"/>
@@ -2712,6 +2755,7 @@
     <hyperlink ref="E56:E60" r:id="rId9" display="Search.png" xr:uid="{226D5616-AE1A-D140-B96F-B62F1F00654E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2719,8 +2763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DC9B6B-62E5-7B4A-80EC-6F20A2BF6C35}">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="116" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView zoomScale="116" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -2729,7 +2773,7 @@
     <col min="2" max="2" width="78" style="11" customWidth="1"/>
     <col min="3" max="3" width="21.83203125" style="11" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="39" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="28" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
@@ -2787,9 +2831,9 @@
         <v>196</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="E5" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="E5" s="26" t="s">
         <v>308</v>
       </c>
     </row>
@@ -2860,7 +2904,7 @@
         <v>150</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>139</v>
+        <v>348</v>
       </c>
       <c r="E12" s="30" t="s">
         <v>306</v>
@@ -2898,7 +2942,7 @@
         <v>151</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>139</v>
+        <v>348</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>199</v>
@@ -2913,7 +2957,7 @@
         <v>152</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>139</v>
+        <v>348</v>
       </c>
       <c r="E16" s="30"/>
     </row>
@@ -3022,7 +3066,7 @@
       <c r="A28" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="27" t="s">
         <v>175</v>
       </c>
       <c r="E28" s="30"/>
@@ -3043,7 +3087,7 @@
       <c r="B30" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="E30" s="35"/>
+      <c r="E30" s="39"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="22" t="s">
@@ -3052,7 +3096,7 @@
       <c r="B31" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="E31" s="35"/>
+      <c r="E31" s="39"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="22" t="s">
@@ -3061,7 +3105,7 @@
       <c r="B32" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="E32" s="35"/>
+      <c r="E32" s="39"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="22" t="s">
@@ -3070,7 +3114,7 @@
       <c r="B33" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="E33" s="35"/>
+      <c r="E33" s="39"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="11" t="s">
@@ -3079,7 +3123,7 @@
       <c r="B34" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="E34" s="34" t="s">
+      <c r="E34" s="26" t="s">
         <v>309</v>
       </c>
     </row>
@@ -3090,7 +3134,7 @@
       <c r="B35" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="E35" s="35"/>
+      <c r="E35" s="39"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="22" t="s">
@@ -3099,7 +3143,7 @@
       <c r="B36" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="E36" s="35"/>
+      <c r="E36" s="39"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="22" t="s">
@@ -3108,7 +3152,7 @@
       <c r="B37" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="E37" s="35"/>
+      <c r="E37" s="39"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="22" t="s">
@@ -3117,7 +3161,7 @@
       <c r="B38" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="E38" s="35"/>
+      <c r="E38" s="39"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="11" t="s">
@@ -3129,18 +3173,18 @@
       <c r="D39" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E39" s="34" t="s">
+      <c r="E39" s="26" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="32" t="s">
         <v>274</v>
       </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="27"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="34"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="11" t="s">
@@ -3150,7 +3194,7 @@
         <v>73</v>
       </c>
       <c r="C41" s="15"/>
-      <c r="E41" s="32" t="s">
+      <c r="E41" s="29" t="s">
         <v>310</v>
       </c>
     </row>
@@ -3212,7 +3256,7 @@
         <v>154</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>155</v>
+        <v>351</v>
       </c>
       <c r="E47" s="30"/>
     </row>
@@ -3224,20 +3268,20 @@
         <v>153</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="E48" s="34" t="s">
+        <v>352</v>
+      </c>
+      <c r="E48" s="26" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="32" t="s">
         <v>275</v>
       </c>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="27"/>
+      <c r="B49" s="33"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="34"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="11" t="s">
@@ -3292,7 +3336,7 @@
         <v>157</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>159</v>
+        <v>349</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -3303,7 +3347,7 @@
         <v>158</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>160</v>
+        <v>350</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -3377,6 +3421,9 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E41:E47"/>
     <mergeCell ref="E8:E11"/>
     <mergeCell ref="E30:E33"/>
     <mergeCell ref="E35:E38"/>
@@ -3384,9 +3431,6 @@
     <mergeCell ref="A49:E49"/>
     <mergeCell ref="E12:E22"/>
     <mergeCell ref="E23:E29"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E41:E47"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E12:E22" r:id="rId1" display="EditTask1.png" xr:uid="{9FE2AE8E-A9CA-964E-A11C-56069919D277}"/>
@@ -3409,7 +3453,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -3539,7 +3583,7 @@
         <v>231</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>139</v>
+        <v>348</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3550,7 +3594,7 @@
         <v>232</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>139</v>
+        <v>348</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>199</v>
@@ -3564,7 +3608,7 @@
         <v>233</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>139</v>
+        <v>348</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3627,8 +3671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53604592-2150-C948-A745-A2773E7BE451}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -3678,7 +3722,7 @@
         <v>230</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>109</v>
+        <v>347</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3689,7 +3733,7 @@
         <v>235</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>139</v>
+        <v>348</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -3717,12 +3761,12 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="32" t="s">
         <v>288</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="27"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="34"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="11" t="s">
@@ -3784,12 +3828,12 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="32" t="s">
         <v>289</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="27"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="34"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="11" t="s">
@@ -3799,7 +3843,7 @@
         <v>252</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>139</v>
+        <v>348</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4143,11 +4187,11 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
       <c r="D13" s="8"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -4270,11 +4314,11 @@
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="9"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -4697,12 +4741,12 @@
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="25" t="s">
+      <c r="A59" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="26"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="27"/>
+      <c r="B59" s="33"/>
+      <c r="C59" s="33"/>
+      <c r="D59" s="34"/>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="11" t="s">
@@ -4783,12 +4827,12 @@
       <c r="D67" s="15"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="25" t="s">
+      <c r="A68" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="B68" s="26"/>
-      <c r="C68" s="26"/>
-      <c r="D68" s="27"/>
+      <c r="B68" s="33"/>
+      <c r="C68" s="33"/>
+      <c r="D68" s="34"/>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="11" t="s">
@@ -4939,10 +4983,10 @@
       <c r="D82" s="15"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="25"/>
-      <c r="B83" s="26"/>
-      <c r="C83" s="26"/>
-      <c r="D83" s="27"/>
+      <c r="A83" s="32"/>
+      <c r="B83" s="33"/>
+      <c r="C83" s="33"/>
+      <c r="D83" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
update test data xpath
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jammytan/Documents/STV-Project/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C43BB2-DBF4-6B4A-BE0A-02A54D66A789}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1283835-B0A4-2943-BF7D-0FFE485262D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="4" r:id="rId1"/>
-    <sheet name="EditTasks_x0009_" sheetId="3" r:id="rId2"/>
+    <sheet name="EditTasks" sheetId="3" r:id="rId2"/>
     <sheet name="ViewTask" sheetId="7" r:id="rId3"/>
     <sheet name="DisplayedLists" sheetId="9" r:id="rId4"/>
     <sheet name="All" sheetId="1" r:id="rId5"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="357">
   <si>
     <t>component</t>
   </si>
@@ -864,28 +864,6 @@
     <t>//*[@text='not specified']</t>
   </si>
   <si>
-    <r>
-      <t>//*[@text='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>${NAME}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>']</t>
-    </r>
-  </si>
-  <si>
     <t>Input field</t>
   </si>
   <si>
@@ -1453,9 +1431,6 @@
     <t>list_delete_list_btn</t>
   </si>
   <si>
-    <t>//*[@class='android.widget.LinearLayout' and ./android.widget.TextView[@text='${NAME}']</t>
-  </si>
-  <si>
     <t>${NAME}</t>
   </si>
   <si>
@@ -1475,7 +1450,7 @@
   </si>
   <si>
     <r>
-      <t>//*[@class='</t>
+      <t>//*[@class='android.widget.LinearLayout' and ./android.widget.TextView[@text='</t>
     </r>
     <r>
       <rPr>
@@ -1483,7 +1458,71 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
+      <t>${NAME}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>//*[@class='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
       <t>android.widget.LinearLayout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' and @index='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${INDEX}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>//*[@class='android.widget.TextView' and @text='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${NAME}</t>
     </r>
     <r>
       <rPr>
@@ -1492,15 +1531,64 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>' and @index='${INDEX}']</t>
-    </r>
+      <t>']</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>//*[@index='4']//*[@resource-id='org.dmfs.tasks:id/checklist']//*[@index='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${INDEX}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']//*[@resource-id='android:id/text1']</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>//*[@index='4']//*[@resource-id='org.dmfs.tasks:id/checklist']//*[@index='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${INDEX}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']//*[@resource-id='android:id/checkbox']</t>
+    </r>
+  </si>
+  <si>
+    <t>//*[@index='11']//*[@class='android.widget.Spinner']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1574,6 +1662,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2092,8 +2185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EF6FCC3-78DA-E74D-BF53-4A0FCE774DC3}">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A12" zoomScale="113" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -2117,10 +2210,10 @@
         <v>106</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2131,7 +2224,7 @@
         <v>61</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2194,7 +2287,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>69</v>
@@ -2206,11 +2299,11 @@
       <c r="A10" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>110</v>
+      <c r="B10" s="14" t="s">
+        <v>353</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E10" s="30"/>
     </row>
@@ -2222,7 +2315,7 @@
         <v>138</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E11" s="30"/>
     </row>
@@ -2231,16 +2324,16 @@
         <v>141</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E12" s="31"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="32" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="33"/>
@@ -2255,7 +2348,7 @@
         <v>70</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2271,11 +2364,11 @@
       <c r="A16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="14" t="s">
-        <v>353</v>
+      <c r="B16" s="11" t="s">
+        <v>352</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E16" s="35"/>
     </row>
@@ -2287,7 +2380,7 @@
         <v>72</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E17" s="35"/>
     </row>
@@ -2311,7 +2404,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="32" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B20" s="33"/>
       <c r="C20" s="33"/>
@@ -2320,18 +2413,18 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>73</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>74</v>
@@ -2340,7 +2433,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="32" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B23" s="33"/>
       <c r="C23" s="33"/>
@@ -2349,45 +2442,45 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E25" s="30"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E26" s="30"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="14" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E27" s="31"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="32" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B28" s="33"/>
       <c r="C28" s="33"/>
@@ -2396,39 +2489,39 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E30" s="30"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E31" s="30"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E32" s="30"/>
     </row>
@@ -2436,17 +2529,17 @@
       <c r="A33" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>110</v>
+      <c r="B33" s="11" t="s">
+        <v>351</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E33" s="31"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="32" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B34" s="33"/>
       <c r="C34" s="33"/>
@@ -2455,49 +2548,49 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C35" s="7"/>
       <c r="E35" s="29" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E36" s="30"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E37" s="30"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E38" s="30"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E39" s="30"/>
     </row>
@@ -2505,17 +2598,17 @@
       <c r="A40" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B40" s="12" t="s">
-        <v>110</v>
+      <c r="B40" s="11" t="s">
+        <v>351</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E40" s="31"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="36" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B41" s="37"/>
       <c r="C41" s="37"/>
@@ -2524,40 +2617,40 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="23" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C42" s="7"/>
       <c r="E42" s="29" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E43" s="30"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E44" s="30"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E45" s="30"/>
     </row>
@@ -2569,7 +2662,7 @@
         <v>138</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E46" s="30"/>
     </row>
@@ -2577,17 +2670,17 @@
       <c r="A47" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B47" s="12" t="s">
-        <v>110</v>
+      <c r="B47" s="11" t="s">
+        <v>351</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E47" s="31"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="32" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B48" s="33"/>
       <c r="C48" s="33"/>
@@ -2596,49 +2689,49 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="23" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C49" s="7"/>
       <c r="E49" s="29" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E50" s="30"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E51" s="30"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="11" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E52" s="30"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E53" s="30"/>
     </row>
@@ -2646,17 +2739,17 @@
       <c r="A54" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B54" s="12" t="s">
-        <v>110</v>
+      <c r="B54" s="11" t="s">
+        <v>351</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E54" s="31"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="32" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B55" s="33"/>
       <c r="C55" s="33"/>
@@ -2665,37 +2758,37 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="23" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E56" s="29" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E57" s="30"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B58" s="14" t="s">
         <v>138</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E58" s="30"/>
     </row>
@@ -2703,11 +2796,11 @@
       <c r="A59" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B59" s="12" t="s">
-        <v>110</v>
+      <c r="B59" s="11" t="s">
+        <v>351</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E59" s="30"/>
     </row>
@@ -2715,11 +2808,11 @@
       <c r="A60" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B60" s="12" t="s">
-        <v>110</v>
+      <c r="B60" s="14" t="s">
+        <v>353</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E60" s="30"/>
     </row>
@@ -2763,8 +2856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DC9B6B-62E5-7B4A-80EC-6F20A2BF6C35}">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView zoomScale="116" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="116" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -2788,10 +2881,10 @@
         <v>107</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2802,12 +2895,12 @@
         <v>76</v>
       </c>
       <c r="E2" s="40" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>67</v>
@@ -2816,7 +2909,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>71</v>
@@ -2827,14 +2920,14 @@
       <c r="A5" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>196</v>
+      <c r="B5" s="11" t="s">
+        <v>352</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2845,15 +2938,15 @@
         <v>80</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>81</v>
@@ -2904,10 +2997,10 @@
         <v>150</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2918,7 +3011,7 @@
         <v>77</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E13" s="30"/>
     </row>
@@ -2930,7 +3023,7 @@
         <v>79</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E14" s="30"/>
     </row>
@@ -2939,13 +3032,13 @@
         <v>39</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>151</v>
+        <v>354</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E15" s="30"/>
     </row>
@@ -2954,10 +3047,10 @@
         <v>40</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>152</v>
+        <v>355</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E16" s="30"/>
     </row>
@@ -3023,12 +3116,12 @@
         <v>84</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>85</v>
@@ -3073,10 +3166,10 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>176</v>
+        <v>356</v>
       </c>
       <c r="E29" s="30"/>
     </row>
@@ -3118,13 +3211,13 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>177</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -3171,15 +3264,15 @@
         <v>178</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="32" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B40" s="33"/>
       <c r="C40" s="33"/>
@@ -3188,19 +3281,19 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>73</v>
       </c>
       <c r="C41" s="15"/>
       <c r="E41" s="29" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>74</v>
@@ -3256,7 +3349,7 @@
         <v>154</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E47" s="30"/>
     </row>
@@ -3268,15 +3361,15 @@
         <v>153</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E48" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="32" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B49" s="33"/>
       <c r="C49" s="33"/>
@@ -3285,7 +3378,7 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B50" s="15" t="s">
         <v>73</v>
@@ -3294,7 +3387,7 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B51" s="15" t="s">
         <v>74</v>
@@ -3336,7 +3429,7 @@
         <v>157</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -3347,7 +3440,7 @@
         <v>158</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -3377,7 +3470,7 @@
       </c>
       <c r="C59" s="15"/>
       <c r="D59" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -3389,12 +3482,12 @@
       </c>
       <c r="C60" s="15"/>
       <c r="D60" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B61" s="15" t="s">
         <v>166</v>
@@ -3453,7 +3546,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -3476,12 +3569,12 @@
         <v>106</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>67</v>
@@ -3489,90 +3582,90 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>201</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>203</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="21" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="21" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="21" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="21" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="20" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3580,10 +3673,10 @@
         <v>40</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3591,53 +3684,53 @@
         <v>39</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>213</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="42" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B20" s="43"/>
       <c r="C20" s="43"/>
@@ -3645,7 +3738,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>73</v>
@@ -3653,7 +3746,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>74</v>
@@ -3672,7 +3765,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -3695,12 +3788,12 @@
         <v>106</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>67</v>
@@ -3708,10 +3801,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>228</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3719,50 +3812,50 @@
         <v>140</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>235</v>
-      </c>
       <c r="C5" s="11" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="33"/>
@@ -3770,18 +3863,18 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>72</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>73</v>
@@ -3789,7 +3882,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>74</v>
@@ -3797,31 +3890,31 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="11" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>74</v>
@@ -3829,7 +3922,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="32" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="33"/>
@@ -3837,58 +3930,58 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>252</v>
-      </c>
       <c r="C18" s="11" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="42" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B24" s="43"/>
       <c r="C24" s="43"/>
@@ -3896,7 +3989,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>73</v>
@@ -3904,7 +3997,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>74</v>
@@ -3955,7 +4048,7 @@
         <v>106</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -4260,7 +4353,7 @@
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>31</v>
@@ -4386,7 +4479,7 @@
         <v>80</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>8</v>
@@ -4511,7 +4604,7 @@
         <v>77</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -4522,7 +4615,7 @@
         <v>79</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -4536,7 +4629,7 @@
         <v>139</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -4737,7 +4830,7 @@
         <v>178</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -4937,7 +5030,7 @@
       </c>
       <c r="C78" s="15"/>
       <c r="D78" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -4949,7 +5042,7 @@
       </c>
       <c r="C79" s="15"/>
       <c r="D79" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="80" spans="1:4">

</xml_diff>

<commit_message>
update editTasks cancel_btn path
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jammytan/Documents/STV-Project/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A47504-B920-1E43-AE48-3EE46F9AA0E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8402A7-254B-DA44-8BC9-B3465B1ED238}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="3" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="4" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="372">
   <si>
     <t>component</t>
   </si>
@@ -1703,6 +1703,9 @@
       </rPr>
       <t>']//*[@resource-id='org.dmfs.tasks:id/btn_settings']</t>
     </r>
+  </si>
+  <si>
+    <t>//*[@resource-id='org.dmfs.tasks:id/action_bar_container']//*[@class='android.widget.ImageButton']</t>
   </si>
 </sst>
 </file>
@@ -2310,8 +2313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EF6FCC3-78DA-E74D-BF53-4A0FCE774DC3}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="109" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -2991,14 +2994,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DC9B6B-62E5-7B4A-80EC-6F20A2BF6C35}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScale="116" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="31" style="11" customWidth="1"/>
-    <col min="2" max="2" width="83" style="11" customWidth="1"/>
+    <col min="2" max="2" width="97.83203125" style="11" customWidth="1"/>
     <col min="3" max="3" width="21.83203125" style="11" customWidth="1"/>
     <col min="4" max="4" width="23.83203125" style="11" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" style="28" customWidth="1"/>
@@ -3037,8 +3040,8 @@
       <c r="A3" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>67</v>
+      <c r="B3" s="12" t="s">
+        <v>371</v>
       </c>
       <c r="E3" s="41"/>
     </row>
@@ -3920,8 +3923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53604592-2150-C948-A745-A2773E7BE451}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="A9" zoomScale="143" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>

</xml_diff>

<commit_message>
update test data pictures
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jammytan/Documents/STV-Project/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8402A7-254B-DA44-8BC9-B3465B1ED238}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1466C0-70D8-FD45-B070-607A89299BD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="4" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="392">
   <si>
     <t>component</t>
   </si>
@@ -1259,9 +1259,6 @@
     <t>status_dropdown</t>
   </si>
   <si>
-    <t>TaskList1.png</t>
-  </si>
-  <si>
     <t>reference</t>
   </si>
   <si>
@@ -1706,6 +1703,69 @@
   </si>
   <si>
     <t>//*[@resource-id='org.dmfs.tasks:id/action_bar_container']//*[@class='android.widget.ImageButton']</t>
+  </si>
+  <si>
+    <t>TaskList.png</t>
+  </si>
+  <si>
+    <t>QuickAddOptions.png</t>
+  </si>
+  <si>
+    <t>Time.png</t>
+  </si>
+  <si>
+    <t>TimeToggleMode.png</t>
+  </si>
+  <si>
+    <t>TimeOptions.png</t>
+  </si>
+  <si>
+    <t>StatusOptions.png</t>
+  </si>
+  <si>
+    <t>PriorityOptions.png</t>
+  </si>
+  <si>
+    <t>PrivacyOptions.png</t>
+  </si>
+  <si>
+    <t>TimezoneOptions.png</t>
+  </si>
+  <si>
+    <t>ViewTask.png</t>
+  </si>
+  <si>
+    <t>ViewTask2.png</t>
+  </si>
+  <si>
+    <t>ConfirmDeleteTask.png</t>
+  </si>
+  <si>
+    <t>ViewTaskMenu.png</t>
+  </si>
+  <si>
+    <t>ViewTaskMenuSeeAll.png</t>
+  </si>
+  <si>
+    <t>ViewTaskMenuCreateTask.png</t>
+  </si>
+  <si>
+    <t>ListSetting.png</t>
+  </si>
+  <si>
+    <t>DisplayedList.png</t>
+  </si>
+  <si>
+    <t>EnterListName.png</t>
+  </si>
+  <si>
+    <t>ConfirmDeleteList.png</t>
+  </si>
+  <si>
+    <t>Synchronize.png</t>
+  </si>
+  <si>
+    <t>PickColor.png</t>
   </si>
 </sst>
 </file>
@@ -1884,7 +1944,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1940,6 +2000,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1974,9 +2037,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1996,6 +2056,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2311,10 +2383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EF6FCC3-78DA-E74D-BF53-4A0FCE774DC3}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56:E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -2323,11 +2395,11 @@
     <col min="2" max="2" width="99.33203125" style="11" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" style="11" customWidth="1"/>
     <col min="4" max="4" width="16.5" style="11" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="11" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="11" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" customHeight="1">
+    <row r="1" spans="1:6" ht="21" customHeight="1">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2341,39 +2413,39 @@
         <v>270</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="29" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2" s="30" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="30"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3" s="31"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="30"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4" s="31"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
@@ -2381,9 +2453,9 @@
         <v>64</v>
       </c>
       <c r="C5" s="12"/>
-      <c r="E5" s="30"/>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="E5" s="31"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
@@ -2391,9 +2463,9 @@
         <v>65</v>
       </c>
       <c r="C6" s="12"/>
-      <c r="E6" s="30"/>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="E6" s="31"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="11" t="s">
         <v>14</v>
       </c>
@@ -2401,9 +2473,9 @@
         <v>66</v>
       </c>
       <c r="C7" s="12"/>
-      <c r="E7" s="30"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E7" s="31"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="22" t="s">
         <v>18</v>
       </c>
@@ -2411,9 +2483,9 @@
         <v>67</v>
       </c>
       <c r="C8" s="12"/>
-      <c r="E8" s="30"/>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="E8" s="31"/>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="11" t="s">
         <v>273</v>
       </c>
@@ -2421,21 +2493,21 @@
         <v>69</v>
       </c>
       <c r="C9" s="12"/>
-      <c r="E9" s="30"/>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E9" s="31"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="11" t="s">
         <v>140</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>343</v>
-      </c>
-      <c r="E10" s="30"/>
-    </row>
-    <row r="11" spans="1:5">
+        <v>342</v>
+      </c>
+      <c r="E10" s="31"/>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
@@ -2443,62 +2515,65 @@
         <v>138</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>344</v>
-      </c>
-      <c r="E11" s="30"/>
-    </row>
-    <row r="12" spans="1:5">
+        <v>343</v>
+      </c>
+      <c r="E11" s="31"/>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>343</v>
-      </c>
-      <c r="E12" s="31"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="E12" s="32"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="33" t="s">
         <v>269</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="34"/>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="35"/>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="11" t="s">
         <v>57</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="35" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="E14" s="47" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="11" t="s">
         <v>56</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="35"/>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="E15" s="36"/>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="11" t="s">
         <v>60</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>343</v>
-      </c>
-      <c r="E16" s="35"/>
+        <v>342</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>372</v>
+      </c>
+      <c r="F16" s="49"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="11" t="s">
@@ -2510,7 +2585,9 @@
       <c r="D17" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E17" s="35"/>
+      <c r="E17" s="36" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
@@ -2519,7 +2596,7 @@
       <c r="B18" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="35"/>
+      <c r="E18" s="36"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
@@ -2528,45 +2605,45 @@
       <c r="B19" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="35"/>
+      <c r="E19" s="48"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="33" t="s">
         <v>284</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="34"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="35"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="29" t="s">
-        <v>291</v>
+      <c r="E21" s="30" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="31"/>
+      <c r="E22" s="32"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="33" t="s">
         <v>279</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="34"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="35"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="14" t="s">
@@ -2575,8 +2652,8 @@
       <c r="B24" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="E24" s="29" t="s">
-        <v>292</v>
+      <c r="E24" s="30" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2586,7 +2663,7 @@
       <c r="B25" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="E25" s="30"/>
+      <c r="E25" s="31"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="14" t="s">
@@ -2595,7 +2672,7 @@
       <c r="B26" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="E26" s="30"/>
+      <c r="E26" s="31"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="14" t="s">
@@ -2604,183 +2681,183 @@
       <c r="B27" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="E27" s="31"/>
+      <c r="E27" s="32"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="33" t="s">
         <v>274</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="34"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="35"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="E29" s="29" t="s">
-        <v>293</v>
+      <c r="E29" s="30" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="E30" s="30"/>
+      <c r="E30" s="31"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="E31" s="30"/>
+      <c r="E31" s="31"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="E32" s="30"/>
+      <c r="E32" s="31"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>343</v>
-      </c>
-      <c r="E33" s="31"/>
+        <v>342</v>
+      </c>
+      <c r="E33" s="32"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="32" t="s">
+      <c r="A34" s="33" t="s">
         <v>275</v>
       </c>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="34"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="35"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="23" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>258</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="E35" s="29" t="s">
-        <v>294</v>
+      <c r="E35" s="30" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="E36" s="30"/>
+      <c r="E36" s="31"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="E37" s="30"/>
+      <c r="E37" s="31"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="E38" s="30"/>
+      <c r="E38" s="31"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="E39" s="30"/>
+      <c r="E39" s="31"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>343</v>
-      </c>
-      <c r="E40" s="31"/>
+        <v>342</v>
+      </c>
+      <c r="E40" s="32"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="37" t="s">
         <v>276</v>
       </c>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="38"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="39"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="23" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>260</v>
       </c>
       <c r="C42" s="7"/>
-      <c r="E42" s="29" t="s">
-        <v>295</v>
+      <c r="E42" s="30" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>361</v>
-      </c>
-      <c r="E43" s="30"/>
+        <v>360</v>
+      </c>
+      <c r="E43" s="31"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>362</v>
-      </c>
-      <c r="E44" s="30"/>
+        <v>361</v>
+      </c>
+      <c r="E44" s="31"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>363</v>
-      </c>
-      <c r="E45" s="30"/>
+        <v>362</v>
+      </c>
+      <c r="E45" s="31"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="11" t="s">
@@ -2790,99 +2867,99 @@
         <v>138</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>344</v>
-      </c>
-      <c r="E46" s="30"/>
+        <v>343</v>
+      </c>
+      <c r="E46" s="31"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>343</v>
-      </c>
-      <c r="E47" s="31"/>
+        <v>342</v>
+      </c>
+      <c r="E47" s="32"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="32" t="s">
+      <c r="A48" s="33" t="s">
         <v>277</v>
       </c>
-      <c r="B48" s="33"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="34"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="35"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="23" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B49" s="11" t="s">
         <v>261</v>
       </c>
       <c r="C49" s="7"/>
-      <c r="E49" s="29" t="s">
-        <v>296</v>
+      <c r="E49" s="30" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B50" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="E50" s="30"/>
+      <c r="E50" s="31"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B51" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="E51" s="30"/>
+      <c r="E51" s="31"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B52" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="E52" s="30"/>
+      <c r="E52" s="31"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B53" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="E53" s="30"/>
+      <c r="E53" s="31"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>343</v>
-      </c>
-      <c r="E54" s="31"/>
+        <v>342</v>
+      </c>
+      <c r="E54" s="32"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="32" t="s">
+      <c r="A55" s="33" t="s">
         <v>278</v>
       </c>
-      <c r="B55" s="33"/>
-      <c r="C55" s="33"/>
-      <c r="D55" s="33"/>
-      <c r="E55" s="34"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="34"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="35"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="23" t="s">
@@ -2895,13 +2972,13 @@
       <c r="D56" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E56" s="29" t="s">
-        <v>299</v>
+      <c r="E56" s="30" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B57" s="15" t="s">
         <v>67</v>
@@ -2911,36 +2988,36 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="E58" s="30"/>
+      <c r="E58" s="31"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>138</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>344</v>
-      </c>
-      <c r="E59" s="30"/>
+        <v>343</v>
+      </c>
+      <c r="E59" s="31"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="14" t="s">
         <v>141</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>343</v>
-      </c>
-      <c r="E60" s="30"/>
+        <v>342</v>
+      </c>
+      <c r="E60" s="31"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="11" t="s">
@@ -2950,20 +3027,21 @@
         <v>196</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>343</v>
-      </c>
-      <c r="E61" s="30"/>
+        <v>342</v>
+      </c>
+      <c r="E61" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="18">
     <mergeCell ref="A55:E55"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E17:E19"/>
     <mergeCell ref="E42:E47"/>
     <mergeCell ref="E49:E54"/>
     <mergeCell ref="E56:E61"/>
     <mergeCell ref="E2:E12"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A20:E20"/>
-    <mergeCell ref="E14:E19"/>
     <mergeCell ref="A23:E23"/>
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="A28:E28"/>
@@ -2977,13 +3055,14 @@
   <hyperlinks>
     <hyperlink ref="E21:E22" r:id="rId1" display="ConfirmDelete.png" xr:uid="{E7D51FE5-38A8-ED48-AB1B-5439A79F0F01}"/>
     <hyperlink ref="E24:E27" r:id="rId2" display="TaskListMenu.png" xr:uid="{41B9DE7C-F513-7A4C-9608-80B8C1A2E0C8}"/>
-    <hyperlink ref="E2:E12" r:id="rId3" display="TaskList1.png" xr:uid="{BEBE0A19-2F55-7C45-BAFA-8F1ED57A8EB4}"/>
-    <hyperlink ref="E14:E19" r:id="rId4" display="QuickAdd.png" xr:uid="{CC8D6B58-F8B3-F44F-A2A2-CA54AEABDA08}"/>
-    <hyperlink ref="E29:E33" r:id="rId5" display="TasksDue.png" xr:uid="{FFDED12F-6E60-764B-AC50-E9A151FE766C}"/>
-    <hyperlink ref="E35:E40" r:id="rId6" display="TasksStarting.png" xr:uid="{D4E49EAD-B8B9-0A49-B1A0-60F7A38DE2EA}"/>
-    <hyperlink ref="E42:E47" r:id="rId7" display="TasksPriority.png" xr:uid="{ABDF668C-400D-2A4E-86EB-E9FD7C44BF55}"/>
-    <hyperlink ref="E49:E54" r:id="rId8" display="TaskProgress.png" xr:uid="{DF68C727-EFA0-7542-B392-52D12BE8F88E}"/>
-    <hyperlink ref="E56:E61" r:id="rId9" display="Search.png" xr:uid="{226D5616-AE1A-D140-B96F-B62F1F00654E}"/>
+    <hyperlink ref="E29:E33" r:id="rId3" display="TasksDue.png" xr:uid="{FFDED12F-6E60-764B-AC50-E9A151FE766C}"/>
+    <hyperlink ref="E35:E40" r:id="rId4" display="TasksStarting.png" xr:uid="{D4E49EAD-B8B9-0A49-B1A0-60F7A38DE2EA}"/>
+    <hyperlink ref="E42:E47" r:id="rId5" display="TasksPriority.png" xr:uid="{ABDF668C-400D-2A4E-86EB-E9FD7C44BF55}"/>
+    <hyperlink ref="E49:E54" r:id="rId6" display="TaskProgress.png" xr:uid="{DF68C727-EFA0-7542-B392-52D12BE8F88E}"/>
+    <hyperlink ref="E56:E61" r:id="rId7" display="Search.png" xr:uid="{226D5616-AE1A-D140-B96F-B62F1F00654E}"/>
+    <hyperlink ref="E2:E12" r:id="rId8" display="TaskList.png" xr:uid="{ED8A8934-31FF-2741-88B1-D7C03C047E87}"/>
+    <hyperlink ref="E17:E19" r:id="rId9" display="QuickAdd.png" xr:uid="{152810F4-07BC-2D49-9C95-15E7C17419AF}"/>
+    <hyperlink ref="E16" r:id="rId10" xr:uid="{8E6C32E5-2FBC-974B-A364-C1B820563A7B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2994,8 +3073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DC9B6B-62E5-7B4A-80EC-6F20A2BF6C35}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -3004,7 +3083,7 @@
     <col min="2" max="2" width="97.83203125" style="11" customWidth="1"/>
     <col min="3" max="3" width="21.83203125" style="11" customWidth="1"/>
     <col min="4" max="4" width="23.83203125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="28" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="29" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
@@ -3022,7 +3101,7 @@
         <v>197</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3033,7 +3112,7 @@
         <v>76</v>
       </c>
       <c r="E2" s="40" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -3041,13 +3120,13 @@
         <v>219</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E3" s="41"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>71</v>
@@ -3059,13 +3138,13 @@
         <v>140</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -3078,8 +3157,8 @@
       <c r="D6" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E6" s="30" t="s">
-        <v>303</v>
+      <c r="E6" s="31" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -3089,16 +3168,18 @@
       <c r="B7" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="30"/>
+      <c r="E7" s="31"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="22" t="s">
         <v>142</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>354</v>
-      </c>
-      <c r="E8" s="30"/>
+        <v>353</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="22" t="s">
@@ -3107,7 +3188,7 @@
       <c r="B9" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="E9" s="30"/>
+      <c r="E9" s="31"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="22" t="s">
@@ -3116,7 +3197,7 @@
       <c r="B10" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="E10" s="30"/>
+      <c r="E10" s="31"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="22" t="s">
@@ -3125,7 +3206,7 @@
       <c r="B11" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="30"/>
+      <c r="E11" s="31"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
@@ -3135,10 +3216,10 @@
         <v>150</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>303</v>
+        <v>343</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3151,7 +3232,7 @@
       <c r="D13" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E13" s="30"/>
+      <c r="E13" s="31"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
@@ -3163,34 +3244,34 @@
       <c r="D14" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E14" s="30"/>
+      <c r="E14" s="31"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E15" s="30"/>
+      <c r="E15" s="31"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="E16" s="30"/>
+        <v>343</v>
+      </c>
+      <c r="E16" s="31"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="11" t="s">
@@ -3199,7 +3280,7 @@
       <c r="B17" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="30"/>
+      <c r="E17" s="31"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
@@ -3208,7 +3289,7 @@
       <c r="B18" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="30"/>
+      <c r="E18" s="31"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
@@ -3217,7 +3298,7 @@
       <c r="B19" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="30"/>
+      <c r="E19" s="31"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
@@ -3226,7 +3307,7 @@
       <c r="B20" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="30"/>
+      <c r="E20" s="31"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
@@ -3235,7 +3316,7 @@
       <c r="B21" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="30"/>
+      <c r="E21" s="31"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
@@ -3244,7 +3325,7 @@
       <c r="B22" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E22" s="30"/>
+      <c r="E22" s="31"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="11" t="s">
@@ -3253,33 +3334,35 @@
       <c r="B23" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="30" t="s">
-        <v>306</v>
+      <c r="E23" s="36" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="30"/>
+      <c r="E24" s="36"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>357</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>358</v>
-      </c>
       <c r="C25" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>360</v>
-      </c>
-      <c r="E25" s="30"/>
+        <v>359</v>
+      </c>
+      <c r="E25" s="50" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="11" t="s">
@@ -3288,7 +3371,9 @@
       <c r="B26" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="30"/>
+      <c r="E26" s="36" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="11" t="s">
@@ -3297,7 +3382,7 @@
       <c r="B27" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="30"/>
+      <c r="E27" s="36"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="11" t="s">
@@ -3306,25 +3391,25 @@
       <c r="B28" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="30"/>
+      <c r="E28" s="36"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="E29" s="30"/>
+      <c r="E29" s="36"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>353</v>
-      </c>
-      <c r="E30" s="30"/>
+        <v>352</v>
+      </c>
+      <c r="E30" s="36"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="22" t="s">
@@ -3333,7 +3418,9 @@
       <c r="B31" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="E31" s="39"/>
+      <c r="E31" s="31" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="22" t="s">
@@ -3342,7 +3429,7 @@
       <c r="B32" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="E32" s="39"/>
+      <c r="E32" s="31"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="22" t="s">
@@ -3351,7 +3438,7 @@
       <c r="B33" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="E33" s="39"/>
+      <c r="E33" s="31"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="22" t="s">
@@ -3360,17 +3447,17 @@
       <c r="B34" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="E34" s="39"/>
+      <c r="E34" s="31"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -3380,7 +3467,9 @@
       <c r="B36" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="E36" s="39"/>
+      <c r="E36" s="31" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="22" t="s">
@@ -3389,7 +3478,7 @@
       <c r="B37" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="E37" s="39"/>
+      <c r="E37" s="31"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="22" t="s">
@@ -3398,7 +3487,7 @@
       <c r="B38" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="E38" s="39"/>
+      <c r="E38" s="31"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="22" t="s">
@@ -3407,52 +3496,52 @@
       <c r="B39" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="E39" s="39"/>
+      <c r="E39" s="31"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
         <v>174</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>199</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="32" t="s">
+      <c r="A41" s="33" t="s">
         <v>271</v>
       </c>
-      <c r="B41" s="33"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="34"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="35"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>73</v>
       </c>
       <c r="C42" s="15"/>
-      <c r="E42" s="29" t="s">
-        <v>307</v>
+      <c r="E42" s="30" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>74</v>
       </c>
       <c r="C43" s="15"/>
-      <c r="E43" s="30"/>
+      <c r="E43" s="31"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="11" t="s">
@@ -3462,7 +3551,7 @@
         <v>95</v>
       </c>
       <c r="C44" s="15"/>
-      <c r="E44" s="30"/>
+      <c r="E44" s="31"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11" t="s">
@@ -3472,7 +3561,7 @@
         <v>96</v>
       </c>
       <c r="C45" s="15"/>
-      <c r="E45" s="30"/>
+      <c r="E45" s="31"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="11" t="s">
@@ -3482,7 +3571,7 @@
         <v>97</v>
       </c>
       <c r="C46" s="15"/>
-      <c r="E46" s="30"/>
+      <c r="E46" s="31"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="11" t="s">
@@ -3492,7 +3581,7 @@
         <v>98</v>
       </c>
       <c r="C47" s="15"/>
-      <c r="E47" s="30"/>
+      <c r="E47" s="31"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="11" t="s">
@@ -3502,9 +3591,9 @@
         <v>154</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>347</v>
-      </c>
-      <c r="E48" s="30"/>
+        <v>346</v>
+      </c>
+      <c r="E48" s="31"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="11" t="s">
@@ -3514,38 +3603,42 @@
         <v>153</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E49" s="26" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="32" t="s">
+      <c r="A50" s="33" t="s">
         <v>272</v>
       </c>
-      <c r="B50" s="33"/>
-      <c r="C50" s="33"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="34"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="34"/>
+      <c r="E50" s="35"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B51" s="15" t="s">
         <v>73</v>
       </c>
       <c r="C51" s="15"/>
+      <c r="E51" s="30" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B52" s="15" t="s">
         <v>74</v>
       </c>
       <c r="C52" s="15"/>
+      <c r="E52" s="31"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="11" t="s">
@@ -3555,6 +3648,7 @@
         <v>101</v>
       </c>
       <c r="C53" s="15"/>
+      <c r="E53" s="31"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="11" t="s">
@@ -3564,6 +3658,7 @@
         <v>102</v>
       </c>
       <c r="C54" s="15"/>
+      <c r="E54" s="31"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="11" t="s">
@@ -3573,6 +3668,7 @@
         <v>103</v>
       </c>
       <c r="C55" s="15"/>
+      <c r="E55" s="31"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="11" t="s">
@@ -3582,8 +3678,9 @@
         <v>157</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>345</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="E56" s="31"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="11" t="s">
@@ -3593,8 +3690,9 @@
         <v>158</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>346</v>
-      </c>
+        <v>345</v>
+      </c>
+      <c r="E57" s="31"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="11" t="s">
@@ -3604,6 +3702,7 @@
         <v>104</v>
       </c>
       <c r="C58" s="15"/>
+      <c r="E58" s="31"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="11" t="s">
@@ -3613,6 +3712,7 @@
         <v>105</v>
       </c>
       <c r="C59" s="15"/>
+      <c r="E59" s="31"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="13" t="s">
@@ -3625,6 +3725,9 @@
       <c r="D60" s="11" t="s">
         <v>198</v>
       </c>
+      <c r="E60" s="31" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="13" t="s">
@@ -3637,15 +3740,17 @@
       <c r="D61" s="11" t="s">
         <v>198</v>
       </c>
+      <c r="E61" s="31"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B62" s="15" t="s">
         <v>166</v>
       </c>
       <c r="C62" s="15"/>
+      <c r="E62" s="31"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="22" t="s">
@@ -3655,6 +3760,9 @@
         <v>169</v>
       </c>
       <c r="C63" s="15"/>
+      <c r="E63" s="31" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="22" t="s">
@@ -3664,30 +3772,43 @@
         <v>170</v>
       </c>
       <c r="C64" s="15"/>
+      <c r="E64" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="E26:E30"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="E42:E48"/>
+    <mergeCell ref="E51:E59"/>
+    <mergeCell ref="E60:E62"/>
     <mergeCell ref="E8:E11"/>
     <mergeCell ref="E31:E34"/>
     <mergeCell ref="E36:E39"/>
     <mergeCell ref="A41:E41"/>
     <mergeCell ref="A50:E50"/>
     <mergeCell ref="E12:E22"/>
-    <mergeCell ref="E23:E30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E12:E22" r:id="rId1" display="EditTask1.png" xr:uid="{9FE2AE8E-A9CA-964E-A11C-56069919D277}"/>
     <hyperlink ref="E2:E4" r:id="rId2" display="EditTask1.png" xr:uid="{AF945763-504F-F44B-941F-F68473F43173}"/>
     <hyperlink ref="E5" r:id="rId3" xr:uid="{C90C6E02-C85B-3048-B0C9-FEDCC070B8E1}"/>
     <hyperlink ref="E6:E7" r:id="rId4" display="EditTask1.png" xr:uid="{7200B3E4-19A9-E34E-B217-AC9A8F0454BD}"/>
-    <hyperlink ref="E23:E30" r:id="rId5" display="EditTask2.png" xr:uid="{1B62641F-1A9C-CA4B-B9EA-354F0B02D7F0}"/>
-    <hyperlink ref="E35" r:id="rId6" xr:uid="{8446D4E4-077D-0A4D-8525-8FB07FF0C373}"/>
-    <hyperlink ref="E40" r:id="rId7" xr:uid="{12FBB57A-780E-814C-87D8-AFBFE84831F1}"/>
-    <hyperlink ref="E42:E48" r:id="rId8" display="Calendar.png" xr:uid="{610945C3-6CA0-044C-8FF8-83DD72D73D6A}"/>
-    <hyperlink ref="E49" r:id="rId9" xr:uid="{7E1BB3A1-2AEF-CA43-9C3D-463F6622F876}"/>
+    <hyperlink ref="E35" r:id="rId5" xr:uid="{8446D4E4-077D-0A4D-8525-8FB07FF0C373}"/>
+    <hyperlink ref="E40" r:id="rId6" xr:uid="{12FBB57A-780E-814C-87D8-AFBFE84831F1}"/>
+    <hyperlink ref="E42:E48" r:id="rId7" display="Calendar.png" xr:uid="{610945C3-6CA0-044C-8FF8-83DD72D73D6A}"/>
+    <hyperlink ref="E49" r:id="rId8" xr:uid="{7E1BB3A1-2AEF-CA43-9C3D-463F6622F876}"/>
+    <hyperlink ref="E51:E59" r:id="rId9" display="Time.png" xr:uid="{AAD316A3-DB94-4240-B398-3FB32A25F9D3}"/>
+    <hyperlink ref="E60:E62" r:id="rId10" display="TimeToggleMode.png" xr:uid="{17A3A39B-02B6-714F-9B1B-FD402BDF5ABA}"/>
+    <hyperlink ref="E63:E64" r:id="rId11" display="TimeOptions.png" xr:uid="{AB6376ED-61CD-AD4E-B9AC-DB5009AA4A5C}"/>
+    <hyperlink ref="E8:E11" r:id="rId12" display="StatusOptions.png" xr:uid="{727B6477-B8DF-D142-8C44-57DAF56E23D5}"/>
+    <hyperlink ref="E31:E34" r:id="rId13" display="PriorityOptions.png" xr:uid="{FDC259CA-E4C3-6746-98E2-92665C5A49E4}"/>
+    <hyperlink ref="E36:E39" r:id="rId14" display="PrivacyOptions.png" xr:uid="{D0EA7266-482F-8D4F-8F27-B9084ABDA77D}"/>
+    <hyperlink ref="E25" r:id="rId15" xr:uid="{ACC8DD5A-7237-0E49-90A1-C93B1602CF73}"/>
+    <hyperlink ref="E23:E24" r:id="rId16" display="EditTask2.png" xr:uid="{E529EFF7-B7A1-524E-A663-6A19E3F92017}"/>
+    <hyperlink ref="E26:E30" r:id="rId17" display="EditTask2.png" xr:uid="{1A63B7F9-20A8-9A47-844C-ED1A1163AB29}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3696,10 +3817,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103321A1-C480-514F-9128-290C60DCE81A}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -3708,10 +3829,12 @@
     <col min="2" max="2" width="123.5" style="11" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" style="11" customWidth="1"/>
     <col min="4" max="4" width="18.83203125" style="11" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="11"/>
+    <col min="5" max="5" width="31.1640625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="11" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -3724,104 +3847,129 @@
       <c r="D1" s="18" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="25" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="20" t="s">
         <v>200</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="30" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="20" t="s">
         <v>201</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="31"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="20" t="s">
         <v>203</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="31"/>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="20" t="s">
         <v>273</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="31"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="21" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="31" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="21" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="31"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="21" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="26" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="21" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="26" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="20" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="31" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="20" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="31"/>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="20" t="s">
         <v>206</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="31"/>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="20" t="s">
         <v>209</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>365</v>
+      </c>
+      <c r="E13" s="31"/>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
         <v>40</v>
       </c>
@@ -3829,10 +3977,11 @@
         <v>229</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>343</v>
+      </c>
+      <c r="E14" s="31"/>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
         <v>39</v>
       </c>
@@ -3840,13 +3989,14 @@
         <v>230</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="31"/>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="46" t="s">
         <v>211</v>
       </c>
@@ -3854,77 +4004,100 @@
         <v>231</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>343</v>
+      </c>
+      <c r="E16" s="31"/>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="20" t="s">
         <v>212</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="31"/>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="20" t="s">
         <v>215</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="31"/>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="20" t="s">
         <v>216</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>367</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="26" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="42" t="s">
         <v>284</v>
       </c>
       <c r="B20" s="43"/>
       <c r="C20" s="43"/>
-      <c r="D20" s="44"/>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="D20" s="43"/>
+      <c r="E20" s="44"/>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="30" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>74</v>
       </c>
+      <c r="E22" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A20:D20"/>
+  <mergeCells count="5">
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E10:E18"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E2:E5" r:id="rId1" display="ViewTask.png" xr:uid="{DBDAF80C-9383-FC40-B83E-398C0807592C}"/>
+    <hyperlink ref="E10:E18" r:id="rId2" display="ViewTask.png" xr:uid="{B769E664-C3A5-C846-8710-7122F377D25C}"/>
+    <hyperlink ref="E19" r:id="rId3" xr:uid="{C5D88C3A-F299-6B4E-A9FD-59313F307545}"/>
+    <hyperlink ref="E21:E22" r:id="rId4" display="ConfirmDeleteTask.png" xr:uid="{4DF7ABBB-AA92-2E44-9C4D-E9A866C1708E}"/>
+    <hyperlink ref="E9" r:id="rId5" xr:uid="{FFBC2EC3-5D16-8D4F-B3A3-FD8D1BDC8A1D}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{5752B374-7244-E240-924D-FA39114A1383}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53604592-2150-C948-A745-A2773E7BE451}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="143" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -3933,10 +4106,11 @@
     <col min="2" max="2" width="113.6640625" style="11" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" style="11" customWidth="1"/>
     <col min="4" max="4" width="14" style="11" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="11"/>
+    <col min="5" max="5" width="21.6640625" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -3949,24 +4123,31 @@
       <c r="D1" s="18" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="17" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="11" t="s">
         <v>200</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="30" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="11" t="s">
         <v>226</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="31"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="11" t="s">
         <v>140</v>
       </c>
@@ -3974,53 +4155,61 @@
         <v>228</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>342</v>
+      </c>
+      <c r="E4" s="31"/>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="11" t="s">
         <v>232</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>343</v>
+      </c>
+      <c r="E5" s="31"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="11" t="s">
         <v>234</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="31"/>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="11" t="s">
         <v>250</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="31" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="11" t="s">
         <v>251</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="32" t="s">
+      <c r="E8" s="32"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="33" t="s">
         <v>285</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="34"/>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="35"/>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="11" t="s">
         <v>235</v>
       </c>
@@ -4030,64 +4219,76 @@
       <c r="D10" s="11" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="30" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="31"/>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="31"/>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="31" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="31"/>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="31"/>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="32" t="s">
+      <c r="E16" s="32"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="33" t="s">
         <v>286</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="34"/>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="35"/>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
         <v>248</v>
       </c>
@@ -4095,79 +4296,106 @@
         <v>249</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>343</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
         <v>243</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="31"/>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
         <v>244</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="31"/>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
         <v>245</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="31"/>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
         <v>246</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" s="31"/>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="11" t="s">
         <v>247</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" s="32"/>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="42" t="s">
         <v>284</v>
       </c>
       <c r="B24" s="43"/>
       <c r="C24" s="43"/>
-      <c r="D24" s="44"/>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="D24" s="43"/>
+      <c r="E24" s="44"/>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" s="30" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>74</v>
       </c>
+      <c r="E26" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A24:D24"/>
+  <mergeCells count="9">
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E2:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="E18:E23"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A24:E24"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E13:E16" r:id="rId1" display="ListSetting.png" xr:uid="{1518F90C-C848-0E46-88B7-B89C8E1E7D4F}"/>
+    <hyperlink ref="E2:E6" r:id="rId2" display="DisplayedList.png" xr:uid="{F7868AFA-E3A6-B44F-AABF-FEA46C17919B}"/>
+    <hyperlink ref="E10:E12" r:id="rId3" display="EnterListName.png" xr:uid="{C73A2777-D611-CD43-B9B4-C3594113B832}"/>
+    <hyperlink ref="E25:E26" r:id="rId4" display="ConfirmDeleteList.png" xr:uid="{BC8B5071-BD9D-AA4A-8E01-D45B59CDDA17}"/>
+    <hyperlink ref="E7:E8" r:id="rId5" display="Synchronize.png" xr:uid="{BC664D47-EA3F-AC44-98C4-CB0A219B6118}"/>
+    <hyperlink ref="E18:E23" r:id="rId6" display="PickColor.png" xr:uid="{BC31547B-6FE5-0843-A8E3-700C667AFBF5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4439,11 +4667,11 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="8"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -4566,11 +4794,11 @@
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
       <c r="D20" s="9"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -4993,12 +5221,12 @@
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="32" t="s">
+      <c r="A59" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="33"/>
-      <c r="C59" s="33"/>
-      <c r="D59" s="34"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="35"/>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="11" t="s">
@@ -5079,12 +5307,12 @@
       <c r="D67" s="15"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="32" t="s">
+      <c r="A68" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="B68" s="33"/>
-      <c r="C68" s="33"/>
-      <c r="D68" s="34"/>
+      <c r="B68" s="34"/>
+      <c r="C68" s="34"/>
+      <c r="D68" s="35"/>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="11" t="s">
@@ -5235,10 +5463,10 @@
       <c r="D82" s="15"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="32"/>
-      <c r="B83" s="33"/>
-      <c r="C83" s="33"/>
-      <c r="D83" s="34"/>
+      <c r="A83" s="33"/>
+      <c r="B83" s="34"/>
+      <c r="C83" s="34"/>
+      <c r="D83" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
add TDS file and Edit End2End Test
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jammytan/Documents/STV-Project/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koushiken/Desktop/Software_Test_Project/STV-Project/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1283835-B0A4-2943-BF7D-0FFE485262D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
+    <workbookView xWindow="6360" yWindow="1880" windowWidth="25600" windowHeight="16000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="4" r:id="rId1"/>
@@ -22,9 +21,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ViewTask!$A$1:$A$10</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -32,12 +37,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>J T</author>
   </authors>
   <commentList>
-    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{DCA326BF-D23A-8941-AD0F-8DD6074573D4}">
+    <comment ref="H10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1587,8 +1592,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1668,6 +1673,14 @@
       <color theme="1"/>
       <name val="Calibri (Body)_x0000_"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1687,14 +1700,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1702,38 +1715,38 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1741,7 +1754,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1751,14 +1764,16 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1820,6 +1835,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1828,15 +1852,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1850,14 +1865,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1869,7 +1884,9 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2182,14 +2199,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EF6FCC3-78DA-E74D-BF53-4A0FCE774DC3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="113" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView zoomScale="113" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" style="11" customWidth="1"/>
     <col min="2" max="2" width="99.33203125" style="11" customWidth="1"/>
@@ -2199,7 +2216,7 @@
     <col min="6" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" customHeight="1">
+    <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2216,36 +2233,36 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="32" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="30"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3" s="33"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="30"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4" s="33"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
@@ -2253,9 +2270,9 @@
         <v>64</v>
       </c>
       <c r="C5" s="12"/>
-      <c r="E5" s="30"/>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="E5" s="33"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
@@ -2263,9 +2280,9 @@
         <v>65</v>
       </c>
       <c r="C6" s="12"/>
-      <c r="E6" s="30"/>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="E6" s="33"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>14</v>
       </c>
@@ -2273,9 +2290,9 @@
         <v>66</v>
       </c>
       <c r="C7" s="12"/>
-      <c r="E7" s="30"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E7" s="33"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>18</v>
       </c>
@@ -2283,9 +2300,9 @@
         <v>67</v>
       </c>
       <c r="C8" s="12"/>
-      <c r="E8" s="30"/>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="E8" s="33"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>275</v>
       </c>
@@ -2293,9 +2310,9 @@
         <v>69</v>
       </c>
       <c r="C9" s="12"/>
-      <c r="E9" s="30"/>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E9" s="33"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>140</v>
       </c>
@@ -2305,9 +2322,9 @@
       <c r="C10" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="E10" s="30"/>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="E10" s="33"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
@@ -2317,9 +2334,9 @@
       <c r="C11" s="14" t="s">
         <v>346</v>
       </c>
-      <c r="E11" s="30"/>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="E11" s="33"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>141</v>
       </c>
@@ -2329,18 +2346,18 @@
       <c r="C12" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="E12" s="31"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="32" t="s">
+      <c r="E12" s="34"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
         <v>271</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="34"/>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="31"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>57</v>
       </c>
@@ -2351,7 +2368,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>56</v>
       </c>
@@ -2360,7 +2377,7 @@
       </c>
       <c r="E15" s="35"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>60</v>
       </c>
@@ -2372,7 +2389,7 @@
       </c>
       <c r="E16" s="35"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>49</v>
       </c>
@@ -2384,7 +2401,7 @@
       </c>
       <c r="E17" s="35"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>48</v>
       </c>
@@ -2393,7 +2410,7 @@
       </c>
       <c r="E18" s="35"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>54</v>
       </c>
@@ -2402,130 +2419,130 @@
       </c>
       <c r="E19" s="35"/>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="32" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
         <v>286</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="34"/>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="31"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>337</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="32" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>338</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="31"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="32" t="s">
+      <c r="E22" s="34"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
         <v>281</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="34"/>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="31"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>282</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="E24" s="29" t="s">
+      <c r="E24" s="32" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>283</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="E25" s="30"/>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="E25" s="33"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>284</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="E26" s="30"/>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="E26" s="33"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>285</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="E27" s="31"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="32" t="s">
+      <c r="E27" s="34"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="29" t="s">
         <v>276</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="34"/>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="31"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>316</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="E29" s="29" t="s">
+      <c r="E29" s="32" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>317</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="E30" s="30"/>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="E30" s="33"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>318</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="E31" s="30"/>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="E31" s="33"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>319</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="E32" s="30"/>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="E32" s="33"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>141</v>
       </c>
@@ -2535,18 +2552,18 @@
       <c r="C33" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="E33" s="31"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="32" t="s">
+      <c r="E33" s="34"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="29" t="s">
         <v>277</v>
       </c>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="34"/>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="31"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>320</v>
       </c>
@@ -2554,47 +2571,47 @@
         <v>260</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="E35" s="29" t="s">
+      <c r="E35" s="32" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>316</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="E36" s="30"/>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="E36" s="33"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>317</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="E37" s="30"/>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="E37" s="33"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>319</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="E38" s="30"/>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="E38" s="33"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>321</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="E39" s="30"/>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="E39" s="33"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>141</v>
       </c>
@@ -2604,9 +2621,9 @@
       <c r="C40" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="E40" s="31"/>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="E40" s="34"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="36" t="s">
         <v>278</v>
       </c>
@@ -2615,7 +2632,7 @@
       <c r="D41" s="37"/>
       <c r="E41" s="38"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
         <v>322</v>
       </c>
@@ -2623,38 +2640,38 @@
         <v>262</v>
       </c>
       <c r="C42" s="7"/>
-      <c r="E42" s="29" t="s">
+      <c r="E42" s="32" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>323</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="E43" s="30"/>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="E43" s="33"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>324</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="E44" s="30"/>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="E44" s="33"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>325</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="E45" s="30"/>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="E45" s="33"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>21</v>
       </c>
@@ -2664,9 +2681,9 @@
       <c r="C46" s="14" t="s">
         <v>346</v>
       </c>
-      <c r="E46" s="30"/>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="E46" s="33"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>141</v>
       </c>
@@ -2676,18 +2693,18 @@
       <c r="C47" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="E47" s="31"/>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="32" t="s">
+      <c r="E47" s="34"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="29" t="s">
         <v>279</v>
       </c>
-      <c r="B48" s="33"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="34"/>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="B48" s="30"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="31"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="23" t="s">
         <v>326</v>
       </c>
@@ -2695,47 +2712,47 @@
         <v>263</v>
       </c>
       <c r="C49" s="7"/>
-      <c r="E49" s="29" t="s">
+      <c r="E49" s="32" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>327</v>
       </c>
       <c r="B50" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="E50" s="30"/>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="E50" s="33"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>328</v>
       </c>
       <c r="B51" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="E51" s="30"/>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="E51" s="33"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>329</v>
       </c>
       <c r="B52" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="E52" s="30"/>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="E52" s="33"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>330</v>
       </c>
       <c r="B53" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="E53" s="30"/>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="E53" s="33"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>141</v>
       </c>
@@ -2745,18 +2762,18 @@
       <c r="C54" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="E54" s="31"/>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="32" t="s">
+      <c r="E54" s="34"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="29" t="s">
         <v>280</v>
       </c>
-      <c r="B55" s="33"/>
-      <c r="C55" s="33"/>
-      <c r="D55" s="33"/>
-      <c r="E55" s="34"/>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="B55" s="30"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="31"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="23" t="s">
         <v>269</v>
       </c>
@@ -2767,20 +2784,20 @@
       <c r="D56" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E56" s="29" t="s">
+      <c r="E56" s="32" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>300</v>
       </c>
       <c r="B57" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="E57" s="30"/>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="E57" s="33"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>299</v>
       </c>
@@ -2790,9 +2807,9 @@
       <c r="C58" s="14" t="s">
         <v>346</v>
       </c>
-      <c r="E58" s="30"/>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="E58" s="33"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>141</v>
       </c>
@@ -2802,9 +2819,9 @@
       <c r="C59" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="E59" s="30"/>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="E59" s="33"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
         <v>140</v>
       </c>
@@ -2814,10 +2831,11 @@
       <c r="C60" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="E60" s="30"/>
+      <c r="E60" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A48:E48"/>
     <mergeCell ref="A55:E55"/>
     <mergeCell ref="E42:E47"/>
     <mergeCell ref="E49:E54"/>
@@ -2834,18 +2852,17 @@
     <mergeCell ref="E29:E33"/>
     <mergeCell ref="A41:E41"/>
     <mergeCell ref="E35:E40"/>
-    <mergeCell ref="A48:E48"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E21:E22" r:id="rId1" display="ConfirmDelete.png" xr:uid="{E7D51FE5-38A8-ED48-AB1B-5439A79F0F01}"/>
-    <hyperlink ref="E24:E27" r:id="rId2" display="TaskListMenu.png" xr:uid="{41B9DE7C-F513-7A4C-9608-80B8C1A2E0C8}"/>
-    <hyperlink ref="E2:E12" r:id="rId3" display="TaskList1.png" xr:uid="{BEBE0A19-2F55-7C45-BAFA-8F1ED57A8EB4}"/>
-    <hyperlink ref="E14:E19" r:id="rId4" display="QuickAdd.png" xr:uid="{CC8D6B58-F8B3-F44F-A2A2-CA54AEABDA08}"/>
-    <hyperlink ref="E29:E33" r:id="rId5" display="TasksDue.png" xr:uid="{FFDED12F-6E60-764B-AC50-E9A151FE766C}"/>
-    <hyperlink ref="E35:E40" r:id="rId6" display="TasksStarting.png" xr:uid="{D4E49EAD-B8B9-0A49-B1A0-60F7A38DE2EA}"/>
-    <hyperlink ref="E42:E47" r:id="rId7" display="TasksPriority.png" xr:uid="{ABDF668C-400D-2A4E-86EB-E9FD7C44BF55}"/>
-    <hyperlink ref="E49:E54" r:id="rId8" display="TaskProgress.png" xr:uid="{DF68C727-EFA0-7542-B392-52D12BE8F88E}"/>
-    <hyperlink ref="E56:E60" r:id="rId9" display="Search.png" xr:uid="{226D5616-AE1A-D140-B96F-B62F1F00654E}"/>
+    <hyperlink ref="E21:E22" r:id="rId1" display="ConfirmDelete.png"/>
+    <hyperlink ref="E24:E27" r:id="rId2" display="TaskListMenu.png"/>
+    <hyperlink ref="E2:E12" r:id="rId3" display="TaskList1.png"/>
+    <hyperlink ref="E14:E19" r:id="rId4" display="QuickAdd.png"/>
+    <hyperlink ref="E29:E33" r:id="rId5" display="TasksDue.png"/>
+    <hyperlink ref="E35:E40" r:id="rId6" display="TasksStarting.png"/>
+    <hyperlink ref="E42:E47" r:id="rId7" display="TasksPriority.png"/>
+    <hyperlink ref="E49:E54" r:id="rId8" display="TaskProgress.png"/>
+    <hyperlink ref="E56:E60" r:id="rId9" display="Search.png"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2853,14 +2870,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DC9B6B-62E5-7B4A-80EC-6F20A2BF6C35}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="116" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="116" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" style="11" customWidth="1"/>
     <col min="2" max="2" width="78" style="11" customWidth="1"/>
@@ -2870,7 +2887,7 @@
     <col min="6" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22" customHeight="1">
+    <row r="1" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2887,36 +2904,36 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="39" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>220</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="41"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3" s="40"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>306</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="41"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4" s="40"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>140</v>
       </c>
@@ -2930,7 +2947,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>32</v>
       </c>
@@ -2940,56 +2957,56 @@
       <c r="D6" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="33" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>289</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="30"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E7" s="33"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>142</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="E8" s="30"/>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="E8" s="33"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>144</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="E9" s="30"/>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E9" s="33"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>146</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="E10" s="30"/>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="E10" s="33"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>148</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="30"/>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="E11" s="33"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>78</v>
       </c>
@@ -2999,11 +3016,11 @@
       <c r="C12" s="11" t="s">
         <v>346</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="33" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>35</v>
       </c>
@@ -3013,9 +3030,9 @@
       <c r="D13" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E13" s="30"/>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="E13" s="33"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>36</v>
       </c>
@@ -3025,9 +3042,9 @@
       <c r="D14" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E14" s="30"/>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="E14" s="33"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>39</v>
       </c>
@@ -3040,9 +3057,9 @@
       <c r="D15" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E15" s="30"/>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="E15" s="33"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>40</v>
       </c>
@@ -3052,164 +3069,164 @@
       <c r="C16" s="11" t="s">
         <v>346</v>
       </c>
-      <c r="E16" s="30"/>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="E16" s="33"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>82</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="30"/>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="E17" s="33"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>112</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="30"/>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="E18" s="33"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>113</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="30"/>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="E19" s="33"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>83</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="30"/>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="E20" s="33"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>114</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="30"/>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="E21" s="33"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>115</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E22" s="30"/>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="E22" s="33"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>116</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E23" s="33" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>304</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="30"/>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="E24" s="33"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>118</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E25" s="30"/>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="E25" s="33"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>119</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E26" s="30"/>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="E26" s="33"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>120</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E27" s="30"/>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="E27" s="33"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>172</v>
       </c>
       <c r="B28" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="E28" s="30"/>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="E28" s="33"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>302</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="E29" s="30"/>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="E29" s="33"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
         <v>180</v>
       </c>
       <c r="B30" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="E30" s="39"/>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="E30" s="41"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
         <v>181</v>
       </c>
       <c r="B31" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="E31" s="39"/>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="E31" s="41"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
         <v>182</v>
       </c>
       <c r="B32" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="E32" s="39"/>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="E32" s="41"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
         <v>183</v>
       </c>
       <c r="B33" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="E33" s="39"/>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="E33" s="41"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>303</v>
       </c>
@@ -3220,43 +3237,43 @@
         <v>308</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
         <v>188</v>
       </c>
       <c r="B35" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="E35" s="39"/>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="E35" s="41"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
         <v>189</v>
       </c>
       <c r="B36" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="E36" s="39"/>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="E36" s="41"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>190</v>
       </c>
       <c r="B37" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="E37" s="39"/>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="E37" s="41"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
         <v>191</v>
       </c>
       <c r="B38" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="E38" s="39"/>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="E38" s="41"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>174</v>
       </c>
@@ -3270,16 +3287,16 @@
         <v>308</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="32" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="29" t="s">
         <v>273</v>
       </c>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="34"/>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="31"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>311</v>
       </c>
@@ -3287,11 +3304,11 @@
         <v>73</v>
       </c>
       <c r="C41" s="15"/>
-      <c r="E41" s="29" t="s">
+      <c r="E41" s="32" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>312</v>
       </c>
@@ -3299,9 +3316,9 @@
         <v>74</v>
       </c>
       <c r="C42" s="15"/>
-      <c r="E42" s="30"/>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="E42" s="33"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>123</v>
       </c>
@@ -3309,9 +3326,9 @@
         <v>95</v>
       </c>
       <c r="C43" s="15"/>
-      <c r="E43" s="30"/>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="E43" s="33"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>124</v>
       </c>
@@ -3319,9 +3336,9 @@
         <v>96</v>
       </c>
       <c r="C44" s="15"/>
-      <c r="E44" s="30"/>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="E44" s="33"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>125</v>
       </c>
@@ -3329,9 +3346,9 @@
         <v>97</v>
       </c>
       <c r="C45" s="15"/>
-      <c r="E45" s="30"/>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="E45" s="33"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>126</v>
       </c>
@@ -3339,9 +3356,9 @@
         <v>98</v>
       </c>
       <c r="C46" s="15"/>
-      <c r="E46" s="30"/>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="E46" s="33"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>127</v>
       </c>
@@ -3351,9 +3368,9 @@
       <c r="C47" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="E47" s="30"/>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="E47" s="33"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>128</v>
       </c>
@@ -3367,16 +3384,16 @@
         <v>310</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="32" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="29" t="s">
         <v>274</v>
       </c>
-      <c r="B49" s="33"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="33"/>
-      <c r="E49" s="34"/>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="B49" s="30"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="31"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>313</v>
       </c>
@@ -3385,7 +3402,7 @@
       </c>
       <c r="C50" s="15"/>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>314</v>
       </c>
@@ -3394,7 +3411,7 @@
       </c>
       <c r="C51" s="15"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>131</v>
       </c>
@@ -3403,7 +3420,7 @@
       </c>
       <c r="C52" s="15"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>132</v>
       </c>
@@ -3412,7 +3429,7 @@
       </c>
       <c r="C53" s="15"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>133</v>
       </c>
@@ -3421,7 +3438,7 @@
       </c>
       <c r="C54" s="15"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>134</v>
       </c>
@@ -3432,7 +3449,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>135</v>
       </c>
@@ -3443,7 +3460,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>136</v>
       </c>
@@ -3452,7 +3469,7 @@
       </c>
       <c r="C57" s="15"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>137</v>
       </c>
@@ -3461,7 +3478,7 @@
       </c>
       <c r="C58" s="15"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>162</v>
       </c>
@@ -3473,7 +3490,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
         <v>161</v>
       </c>
@@ -3485,7 +3502,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
         <v>315</v>
       </c>
@@ -3494,7 +3511,7 @@
       </c>
       <c r="C61" s="15"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="22" t="s">
         <v>167</v>
       </c>
@@ -3503,7 +3520,7 @@
       </c>
       <c r="C62" s="15"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="22" t="s">
         <v>168</v>
       </c>
@@ -3514,6 +3531,9 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="E12:E22"/>
+    <mergeCell ref="E23:E29"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="E41:E47"/>
@@ -3521,20 +3541,17 @@
     <mergeCell ref="E30:E33"/>
     <mergeCell ref="E35:E38"/>
     <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="E12:E22"/>
-    <mergeCell ref="E23:E29"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E12:E22" r:id="rId1" display="EditTask1.png" xr:uid="{9FE2AE8E-A9CA-964E-A11C-56069919D277}"/>
-    <hyperlink ref="E2:E4" r:id="rId2" display="EditTask1.png" xr:uid="{AF945763-504F-F44B-941F-F68473F43173}"/>
-    <hyperlink ref="E5" r:id="rId3" xr:uid="{C90C6E02-C85B-3048-B0C9-FEDCC070B8E1}"/>
-    <hyperlink ref="E6:E7" r:id="rId4" display="EditTask1.png" xr:uid="{7200B3E4-19A9-E34E-B217-AC9A8F0454BD}"/>
-    <hyperlink ref="E23:E29" r:id="rId5" display="EditTask2.png" xr:uid="{1B62641F-1A9C-CA4B-B9EA-354F0B02D7F0}"/>
-    <hyperlink ref="E34" r:id="rId6" xr:uid="{8446D4E4-077D-0A4D-8525-8FB07FF0C373}"/>
-    <hyperlink ref="E39" r:id="rId7" xr:uid="{12FBB57A-780E-814C-87D8-AFBFE84831F1}"/>
-    <hyperlink ref="E41:E47" r:id="rId8" display="Calendar.png" xr:uid="{610945C3-6CA0-044C-8FF8-83DD72D73D6A}"/>
-    <hyperlink ref="E48" r:id="rId9" xr:uid="{7E1BB3A1-2AEF-CA43-9C3D-463F6622F876}"/>
+    <hyperlink ref="E12:E22" r:id="rId1" display="EditTask1.png"/>
+    <hyperlink ref="E2:E4" r:id="rId2" display="EditTask1.png"/>
+    <hyperlink ref="E5" r:id="rId3"/>
+    <hyperlink ref="E6:E7" r:id="rId4" display="EditTask1.png"/>
+    <hyperlink ref="E23:E29" r:id="rId5" display="EditTask2.png"/>
+    <hyperlink ref="E34" r:id="rId6"/>
+    <hyperlink ref="E39" r:id="rId7"/>
+    <hyperlink ref="E41:E47" r:id="rId8" display="Calendar.png"/>
+    <hyperlink ref="E48" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3542,14 +3559,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103321A1-C480-514F-9128-290C60DCE81A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.83203125" style="20" customWidth="1"/>
     <col min="2" max="2" width="118.6640625" style="11" customWidth="1"/>
@@ -3558,7 +3575,7 @@
     <col min="5" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -3572,7 +3589,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>199</v>
       </c>
@@ -3580,7 +3597,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>200</v>
       </c>
@@ -3588,7 +3605,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>202</v>
       </c>
@@ -3596,7 +3613,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>275</v>
       </c>
@@ -3604,7 +3621,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>331</v>
       </c>
@@ -3612,7 +3629,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>332</v>
       </c>
@@ -3620,7 +3637,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>333</v>
       </c>
@@ -3628,7 +3645,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>334</v>
       </c>
@@ -3636,7 +3653,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>335</v>
       </c>
@@ -3644,7 +3661,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>336</v>
       </c>
@@ -3652,7 +3669,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>205</v>
       </c>
@@ -3660,7 +3677,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>209</v>
       </c>
@@ -3668,7 +3685,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>40</v>
       </c>
@@ -3679,7 +3696,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>39</v>
       </c>
@@ -3693,7 +3710,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>211</v>
       </c>
@@ -3704,7 +3721,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>212</v>
       </c>
@@ -3712,7 +3729,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>215</v>
       </c>
@@ -3720,7 +3737,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>217</v>
       </c>
@@ -3728,7 +3745,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="42" t="s">
         <v>286</v>
       </c>
@@ -3736,7 +3753,7 @@
       <c r="C20" s="43"/>
       <c r="D20" s="44"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>337</v>
       </c>
@@ -3744,7 +3761,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>338</v>
       </c>
@@ -3761,14 +3778,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53604592-2150-C948-A745-A2773E7BE451}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.6640625" style="11" customWidth="1"/>
     <col min="2" max="2" width="113.6640625" style="11" customWidth="1"/>
@@ -3777,7 +3794,7 @@
     <col min="5" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -3791,7 +3808,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>199</v>
       </c>
@@ -3799,7 +3816,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>227</v>
       </c>
@@ -3807,7 +3824,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>140</v>
       </c>
@@ -3818,7 +3835,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>233</v>
       </c>
@@ -3829,7 +3846,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>236</v>
       </c>
@@ -3837,7 +3854,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>252</v>
       </c>
@@ -3845,7 +3862,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>253</v>
       </c>
@@ -3853,15 +3870,15 @@
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="32" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
         <v>287</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="34"/>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="31"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>237</v>
       </c>
@@ -3872,7 +3889,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>339</v>
       </c>
@@ -3880,7 +3897,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>340</v>
       </c>
@@ -3888,7 +3905,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>341</v>
       </c>
@@ -3896,7 +3913,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>342</v>
       </c>
@@ -3904,7 +3921,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>343</v>
       </c>
@@ -3912,7 +3929,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>344</v>
       </c>
@@ -3920,15 +3937,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="32" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
         <v>288</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="34"/>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="31"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>250</v>
       </c>
@@ -3939,7 +3956,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>245</v>
       </c>
@@ -3947,7 +3964,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>246</v>
       </c>
@@ -3955,7 +3972,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>247</v>
       </c>
@@ -3963,7 +3980,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>248</v>
       </c>
@@ -3971,7 +3988,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>249</v>
       </c>
@@ -3979,7 +3996,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="42" t="s">
         <v>286</v>
       </c>
@@ -3987,7 +4004,7 @@
       <c r="C24" s="43"/>
       <c r="D24" s="44"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>337</v>
       </c>
@@ -3995,7 +4012,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>338</v>
       </c>
@@ -4014,14 +4031,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296F9A35-BE5A-E64F-9080-864E7183DD30}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.33203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="107.6640625" style="11" customWidth="1"/>
@@ -4037,7 +4054,7 @@
     <col min="12" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="33" customHeight="1">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -4072,7 +4089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
@@ -4089,7 +4106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
@@ -4106,7 +4123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
@@ -4123,7 +4140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
@@ -4142,7 +4159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
@@ -4161,7 +4178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>14</v>
       </c>
@@ -4180,7 +4197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>18</v>
       </c>
@@ -4199,7 +4216,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
@@ -4215,7 +4232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -4233,7 +4250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
@@ -4257,7 +4274,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>26</v>
       </c>
@@ -4279,12 +4296,12 @@
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="32" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="8"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -4294,7 +4311,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>57</v>
       </c>
@@ -4311,7 +4328,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>56</v>
       </c>
@@ -4328,7 +4345,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>60</v>
       </c>
@@ -4344,7 +4361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>49</v>
       </c>
@@ -4368,7 +4385,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>48</v>
       </c>
@@ -4387,7 +4404,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>54</v>
       </c>
@@ -4406,7 +4423,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="36" t="s">
         <v>59</v>
       </c>
@@ -4421,7 +4438,7 @@
       <c r="J20" s="4"/>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>28</v>
       </c>
@@ -4435,7 +4452,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>111</v>
       </c>
@@ -4443,7 +4460,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>30</v>
       </c>
@@ -4457,7 +4474,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>37</v>
       </c>
@@ -4471,7 +4488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>32</v>
       </c>
@@ -4491,7 +4508,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>34</v>
       </c>
@@ -4508,7 +4525,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>142</v>
       </c>
@@ -4516,7 +4533,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>144</v>
       </c>
@@ -4533,7 +4550,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>146</v>
       </c>
@@ -4550,7 +4567,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>148</v>
       </c>
@@ -4573,7 +4590,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>78</v>
       </c>
@@ -4596,7 +4613,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>35</v>
       </c>
@@ -4607,7 +4624,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>36</v>
       </c>
@@ -4618,7 +4635,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>39</v>
       </c>
@@ -4632,7 +4649,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>40</v>
       </c>
@@ -4643,7 +4660,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>82</v>
       </c>
@@ -4651,7 +4668,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>112</v>
       </c>
@@ -4659,7 +4676,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>113</v>
       </c>
@@ -4667,7 +4684,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>83</v>
       </c>
@@ -4675,7 +4692,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>114</v>
       </c>
@@ -4683,7 +4700,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>115</v>
       </c>
@@ -4691,7 +4708,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>116</v>
       </c>
@@ -4699,7 +4716,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>117</v>
       </c>
@@ -4707,7 +4724,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>118</v>
       </c>
@@ -4715,7 +4732,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>119</v>
       </c>
@@ -4723,7 +4740,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>120</v>
       </c>
@@ -4731,7 +4748,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>172</v>
       </c>
@@ -4742,7 +4759,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>171</v>
       </c>
@@ -4750,7 +4767,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>180</v>
       </c>
@@ -4758,7 +4775,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>181</v>
       </c>
@@ -4766,7 +4783,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>182</v>
       </c>
@@ -4774,7 +4791,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>183</v>
       </c>
@@ -4782,7 +4799,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>173</v>
       </c>
@@ -4790,7 +4807,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>188</v>
       </c>
@@ -4798,7 +4815,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>189</v>
       </c>
@@ -4806,7 +4823,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>190</v>
       </c>
@@ -4814,7 +4831,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>191</v>
       </c>
@@ -4822,7 +4839,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>174</v>
       </c>
@@ -4833,15 +4850,15 @@
         <v>198</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="32" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="33"/>
-      <c r="C59" s="33"/>
-      <c r="D59" s="34"/>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="B59" s="30"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="31"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
         <v>121</v>
       </c>
@@ -4849,7 +4866,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
         <v>122</v>
       </c>
@@ -4857,7 +4874,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
         <v>123</v>
       </c>
@@ -4865,7 +4882,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
         <v>124</v>
       </c>
@@ -4875,7 +4892,7 @@
       <c r="C63" s="15"/>
       <c r="D63" s="15"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
         <v>125</v>
       </c>
@@ -4885,7 +4902,7 @@
       <c r="C64" s="15"/>
       <c r="D64" s="15"/>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
         <v>126</v>
       </c>
@@ -4895,7 +4912,7 @@
       <c r="C65" s="15"/>
       <c r="D65" s="15"/>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
         <v>127</v>
       </c>
@@ -4907,7 +4924,7 @@
       </c>
       <c r="D66" s="15"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
         <v>128</v>
       </c>
@@ -4919,15 +4936,15 @@
       </c>
       <c r="D67" s="15"/>
     </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="32" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="B68" s="33"/>
-      <c r="C68" s="33"/>
-      <c r="D68" s="34"/>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="B68" s="30"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="31"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
         <v>129</v>
       </c>
@@ -4937,7 +4954,7 @@
       <c r="C69" s="15"/>
       <c r="D69" s="15"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
         <v>130</v>
       </c>
@@ -4947,7 +4964,7 @@
       <c r="C70" s="15"/>
       <c r="D70" s="15"/>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
         <v>131</v>
       </c>
@@ -4957,7 +4974,7 @@
       <c r="C71" s="15"/>
       <c r="D71" s="15"/>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>132</v>
       </c>
@@ -4967,7 +4984,7 @@
       <c r="C72" s="15"/>
       <c r="D72" s="15"/>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>133</v>
       </c>
@@ -4977,7 +4994,7 @@
       <c r="C73" s="15"/>
       <c r="D73" s="15"/>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>134</v>
       </c>
@@ -4989,7 +5006,7 @@
       </c>
       <c r="D74" s="15"/>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
         <v>135</v>
       </c>
@@ -5001,7 +5018,7 @@
       </c>
       <c r="D75" s="15"/>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
         <v>136</v>
       </c>
@@ -5011,7 +5028,7 @@
       <c r="C76" s="15"/>
       <c r="D76" s="15"/>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>137</v>
       </c>
@@ -5021,7 +5038,7 @@
       <c r="C77" s="15"/>
       <c r="D77" s="15"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
         <v>162</v>
       </c>
@@ -5033,7 +5050,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
         <v>161</v>
       </c>
@@ -5045,7 +5062,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
         <v>165</v>
       </c>
@@ -5055,7 +5072,7 @@
       <c r="C80" s="15"/>
       <c r="D80" s="15"/>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
         <v>167</v>
       </c>
@@ -5065,7 +5082,7 @@
       <c r="C81" s="15"/>
       <c r="D81" s="15"/>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
         <v>168</v>
       </c>
@@ -5075,11 +5092,11 @@
       <c r="C82" s="15"/>
       <c r="D82" s="15"/>
     </row>
-    <row r="83" spans="1:4">
-      <c r="A83" s="32"/>
-      <c r="B83" s="33"/>
-      <c r="C83" s="33"/>
-      <c r="D83" s="34"/>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="29"/>
+      <c r="B83" s="30"/>
+      <c r="C83" s="30"/>
+      <c r="D83" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>